<commit_message>
Homework 5 - Q1 & Q2 Updated
</commit_message>
<xml_diff>
--- a/Assignment 3 Color Opponency/HW_Opponency_Data.xlsx
+++ b/Assignment 3 Color Opponency/HW_Opponency_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmpocs/Google Drive mmpocs/Course 601 Principles/Homework Mike/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pratheepkumarc/Documents/Development/Matlab/Principles-of-Color-Science/Assignment 3 Color Opponency/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F4F011-9F7E-4645-A9C5-74139A2D3917}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACDD154C-05DC-5F43-8E49-9B40BC33978E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35080" yWindow="-4600" windowWidth="27840" windowHeight="19180" activeTab="1" xr2:uid="{E41CB8FE-F870-7743-B367-85CF2576C8CB}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="1" xr2:uid="{E41CB8FE-F870-7743-B367-85CF2576C8CB}"/>
   </bookViews>
   <sheets>
     <sheet name="ColorChecker" sheetId="3" r:id="rId1"/>
@@ -2114,7 +2114,7 @@
   <dimension ref="A1:Y37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4978,7 +4978,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39:D39"/>
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5509,7 +5509,7 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B39" sqref="B39:C39"/>
+      <selection activeCell="B2" sqref="B2:B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Assignment 14 - Report Updated
</commit_message>
<xml_diff>
--- a/Assignment 3 Color Opponency/HW_Opponency_Data.xlsx
+++ b/Assignment 3 Color Opponency/HW_Opponency_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pratheepkumarc/Documents/Development/Matlab/Principles-of-Color-Science/Assignment 3 Color Opponency/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACDD154C-05DC-5F43-8E49-9B40BC33978E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{961839C6-E809-0342-802B-79EEAD8D5158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="1" xr2:uid="{E41CB8FE-F870-7743-B367-85CF2576C8CB}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19980" xr2:uid="{E41CB8FE-F870-7743-B367-85CF2576C8CB}"/>
   </bookViews>
   <sheets>
     <sheet name="ColorChecker" sheetId="3" r:id="rId1"/>
@@ -2113,8 +2113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{114BF304-BFCC-D942-91CE-26FE669DE621}">
   <dimension ref="A1:Y37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T45" sqref="T45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4977,7 +4977,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02EB5BDB-D16D-C743-BA8B-75B48DD4B63A}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
@@ -5508,8 +5508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E764E4B-E059-6C41-8D54-72921272F57D}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B37"/>
+    <sheetView topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>